<commit_message>
Funciones de element en el DOM
</commit_message>
<xml_diff>
--- a/documentacion/03 - ANEXO - Historias de Usuario Simplificada - EJEMPLO.xlsx
+++ b/documentacion/03 - ANEXO - Historias de Usuario Simplificada - EJEMPLO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodiGo\codigo-virtual-3\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F693A92-0702-4093-9C2D-A87A19A5F570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9A12C-2E43-4027-AF15-11D7DE8354E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -173,13 +173,16 @@
   </si>
   <si>
     <t>Peso</t>
+  </si>
+  <si>
+    <t>PRODUCT BACKLOG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +244,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -289,7 +300,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -301,6 +312,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -646,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -657,14 +669,15 @@
     <col min="1" max="1" width="6.375" customWidth="1"/>
     <col min="2" max="2" width="51.875" customWidth="1"/>
     <col min="3" max="3" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21">
+    <row r="2" spans="1:6" ht="21">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -678,7 +691,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="47.25">
+    <row r="3" spans="1:6" ht="47.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -692,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="47.25">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -705,8 +718,11 @@
       <c r="D4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="63">
+      <c r="F4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="63">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -720,7 +736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="94.5">
+    <row r="6" spans="1:6" ht="94.5">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -734,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="141.75">
+    <row r="7" spans="1:6" ht="141.75">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -748,7 +764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="110.25">
+    <row r="8" spans="1:6" ht="110.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -762,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="78.75">
+    <row r="9" spans="1:6" ht="78.75">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -776,7 +792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -784,7 +800,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -792,7 +808,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -800,7 +816,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -808,7 +824,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -816,7 +832,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -824,7 +840,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>